<commit_message>
revisions to performance matrix following dicussion with JC/HA
</commit_message>
<xml_diff>
--- a/data/raw/Performance-Matrix-RW.xlsx
+++ b/data/raw/Performance-Matrix-RW.xlsx
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3302" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3302" uniqueCount="1031">
   <si>
     <t>knee, hip or both filter (1/0/10)</t>
   </si>
@@ -4069,6 +4069,9 @@
   </si>
   <si>
     <t>$17,290-$30,600</t>
+  </si>
+  <si>
+    <t>-0.64 [-0.95, -0.33]</t>
   </si>
 </sst>
 </file>
@@ -4497,9 +4500,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4524,6 +4524,9 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -4532,317 +4535,7 @@
     <cellStyle name="Normal 2" xfId="4"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="295">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="264">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7794,13 +7487,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AR141"/>
+  <dimension ref="A1:AQ141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R114" sqref="R114"/>
+      <selection pane="bottomRight" activeCell="A83" sqref="A83:XFD83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -7815,13 +7508,13 @@
     <col min="11" max="15" width="4" style="95" customWidth="1"/>
     <col min="16" max="16" width="10" style="15" customWidth="1"/>
     <col min="17" max="17" width="5.5703125" style="15" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" style="106" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" style="105" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="33.85546875" style="15" customWidth="1"/>
     <col min="21" max="21" width="11.28515625" style="17" customWidth="1"/>
     <col min="22" max="25" width="12" style="15" customWidth="1"/>
     <col min="26" max="26" width="8.85546875" style="15" customWidth="1"/>
-    <col min="27" max="27" width="20.7109375" style="106" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.7109375" style="105" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="26.5703125" style="59" customWidth="1"/>
     <col min="29" max="29" width="13.140625" style="59" customWidth="1"/>
     <col min="30" max="30" width="21.5703125" style="15" customWidth="1"/>
@@ -7831,7 +7524,7 @@
     <col min="35" max="36" width="18.5703125" style="15" customWidth="1"/>
     <col min="37" max="37" width="26.85546875" style="19" customWidth="1"/>
     <col min="38" max="38" width="11.42578125" style="13" customWidth="1"/>
-    <col min="39" max="39" width="17.85546875" style="111" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.85546875" style="110" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="22.5703125" style="15" customWidth="1"/>
     <col min="41" max="41" width="10.5703125" style="13" customWidth="1"/>
     <col min="42" max="42" width="17.42578125" style="15" customWidth="1"/>
@@ -7870,20 +7563,20 @@
       <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="104" t="s">
+      <c r="K1" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="104"/>
-      <c r="M1" s="104"/>
-      <c r="N1" s="104"/>
-      <c r="O1" s="104"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
       <c r="P1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="105"/>
+      <c r="R1" s="104"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6" t="s">
         <v>13</v>
@@ -7906,7 +7599,7 @@
       <c r="Z1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="110"/>
+      <c r="AA1" s="109"/>
       <c r="AB1" s="8" t="s">
         <v>20</v>
       </c>
@@ -7940,7 +7633,7 @@
       <c r="AL1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="113"/>
+      <c r="AM1" s="112"/>
       <c r="AN1" s="1" t="s">
         <v>31</v>
       </c>
@@ -8001,7 +7694,7 @@
       <c r="Q2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="105" t="s">
+      <c r="R2" s="104" t="s">
         <v>953</v>
       </c>
       <c r="S2" s="6" t="s">
@@ -8016,7 +7709,7 @@
       <c r="Z2" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="110" t="s">
+      <c r="AA2" s="109" t="s">
         <v>990</v>
       </c>
       <c r="AB2" s="8"/>
@@ -8032,7 +7725,7 @@
       <c r="AL2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="AM2" s="113" t="s">
+      <c r="AM2" s="112" t="s">
         <v>1015</v>
       </c>
       <c r="AO2" s="11" t="s">
@@ -8053,7 +7746,7 @@
       <c r="O3" s="15"/>
       <c r="P3" s="16"/>
       <c r="Z3" s="13"/>
-      <c r="AA3" s="111"/>
+      <c r="AA3" s="110"/>
       <c r="AB3" s="17"/>
       <c r="AC3" s="17"/>
       <c r="AD3" s="16"/>
@@ -8105,7 +7798,7 @@
       <c r="Q4" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R4" s="106" t="s">
+      <c r="R4" s="105" t="s">
         <v>956</v>
       </c>
       <c r="T4" s="21" t="s">
@@ -8129,7 +7822,7 @@
       <c r="Z4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA4" s="111" t="s">
+      <c r="AA4" s="110" t="s">
         <v>991</v>
       </c>
       <c r="AB4" s="17" t="s">
@@ -8165,7 +7858,7 @@
       <c r="AL4" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM4" s="114" t="s">
+      <c r="AM4" s="113" t="s">
         <v>73</v>
       </c>
       <c r="AN4" s="28" t="s">
@@ -8332,7 +8025,7 @@
       <c r="Q6" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R6" s="106" t="s">
+      <c r="R6" s="105" t="s">
         <v>956</v>
       </c>
       <c r="T6" s="25" t="s">
@@ -8356,7 +8049,7 @@
       <c r="Z6" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA6" s="111" t="s">
+      <c r="AA6" s="110" t="s">
         <v>991</v>
       </c>
       <c r="AB6" s="13" t="s">
@@ -8392,7 +8085,7 @@
       <c r="AL6" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM6" s="114" t="s">
+      <c r="AM6" s="113" t="s">
         <v>94</v>
       </c>
       <c r="AN6" s="28" t="s">
@@ -8559,7 +8252,7 @@
       <c r="Q8" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R8" s="106" t="s">
+      <c r="R8" s="105" t="s">
         <v>957</v>
       </c>
       <c r="T8" s="33" t="s">
@@ -8583,7 +8276,7 @@
       <c r="Z8" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA8" s="111" t="s">
+      <c r="AA8" s="110" t="s">
         <v>992</v>
       </c>
       <c r="AB8" s="12" t="s">
@@ -8616,7 +8309,7 @@
       <c r="AL8" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM8" s="114" t="s">
+      <c r="AM8" s="113" t="s">
         <v>112</v>
       </c>
       <c r="AN8" s="28" t="s">
@@ -8671,7 +8364,7 @@
       <c r="Q9" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R9" s="106" t="s">
+      <c r="R9" s="105" t="s">
         <v>957</v>
       </c>
       <c r="T9" s="15" t="s">
@@ -8695,7 +8388,7 @@
       <c r="Z9" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA9" s="111" t="s">
+      <c r="AA9" s="110" t="s">
         <v>992</v>
       </c>
       <c r="AB9" s="15" t="s">
@@ -8725,8 +8418,8 @@
       <c r="AL9" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AM9" s="114" t="s">
-        <v>119</v>
+      <c r="AM9" s="113" t="s">
+        <v>1030</v>
       </c>
       <c r="AN9" s="39" t="s">
         <v>120</v>
@@ -8780,7 +8473,7 @@
       <c r="Q10" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="106" t="s">
+      <c r="R10" s="105" t="s">
         <v>957</v>
       </c>
       <c r="T10" s="15" t="s">
@@ -8804,7 +8497,7 @@
       <c r="Z10" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA10" s="111" t="s">
+      <c r="AA10" s="110" t="s">
         <v>992</v>
       </c>
       <c r="AB10" s="15" t="s">
@@ -8834,7 +8527,7 @@
       <c r="AL10" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AM10" s="114" t="s">
+      <c r="AM10" s="113" t="s">
         <v>123</v>
       </c>
       <c r="AN10" s="39" t="s">
@@ -8889,7 +8582,7 @@
       <c r="Q11" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R11" s="106" t="s">
+      <c r="R11" s="105" t="s">
         <v>957</v>
       </c>
       <c r="T11" s="15" t="s">
@@ -8913,7 +8606,7 @@
       <c r="Z11" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA11" s="111" t="s">
+      <c r="AA11" s="110" t="s">
         <v>992</v>
       </c>
       <c r="AB11" s="15" t="s">
@@ -8946,7 +8639,7 @@
       <c r="AL11" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM11" s="114" t="s">
+      <c r="AM11" s="113" t="s">
         <v>128</v>
       </c>
       <c r="AN11" s="39" t="s">
@@ -9001,7 +8694,7 @@
       <c r="Q12" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R12" s="106" t="s">
+      <c r="R12" s="105" t="s">
         <v>957</v>
       </c>
       <c r="T12" s="15" t="s">
@@ -9025,7 +8718,7 @@
       <c r="Z12" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA12" s="111" t="s">
+      <c r="AA12" s="110" t="s">
         <v>992</v>
       </c>
       <c r="AB12" s="15" t="s">
@@ -9058,7 +8751,7 @@
       <c r="AL12" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM12" s="114" t="s">
+      <c r="AM12" s="113" t="s">
         <v>134</v>
       </c>
       <c r="AN12" s="40" t="s">
@@ -9116,7 +8809,7 @@
       <c r="Q13" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R13" s="106" t="s">
+      <c r="R13" s="105" t="s">
         <v>957</v>
       </c>
       <c r="T13" s="15" t="s">
@@ -9140,7 +8833,7 @@
       <c r="Z13" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA13" s="111" t="s">
+      <c r="AA13" s="110" t="s">
         <v>993</v>
       </c>
       <c r="AB13" s="17" t="s">
@@ -9173,7 +8866,7 @@
       <c r="AL13" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AM13" s="114" t="s">
+      <c r="AM13" s="113" t="s">
         <v>140</v>
       </c>
       <c r="AN13" s="39" t="s">
@@ -9228,7 +8921,7 @@
       <c r="Q14" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R14" s="106" t="s">
+      <c r="R14" s="105" t="s">
         <v>957</v>
       </c>
       <c r="T14" s="15" t="s">
@@ -9252,7 +8945,7 @@
       <c r="Z14" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA14" s="111" t="s">
+      <c r="AA14" s="110" t="s">
         <v>992</v>
       </c>
       <c r="AB14" s="15" t="s">
@@ -9285,7 +8978,7 @@
       <c r="AL14" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM14" s="114" t="s">
+      <c r="AM14" s="113" t="s">
         <v>145</v>
       </c>
       <c r="AN14" s="41" t="s">
@@ -9343,7 +9036,7 @@
       <c r="Q15" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R15" s="106" t="s">
+      <c r="R15" s="105" t="s">
         <v>957</v>
       </c>
       <c r="T15" s="15" t="s">
@@ -9367,7 +9060,7 @@
       <c r="Z15" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA15" s="111" t="s">
+      <c r="AA15" s="110" t="s">
         <v>992</v>
       </c>
       <c r="AB15" s="15" t="s">
@@ -9403,7 +9096,7 @@
       <c r="AL15" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM15" s="114"/>
+      <c r="AM15" s="113"/>
       <c r="AN15" s="19" t="s">
         <v>149</v>
       </c>
@@ -10101,7 +9794,7 @@
       <c r="Q22" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R22" s="106" t="s">
+      <c r="R22" s="105" t="s">
         <v>958</v>
       </c>
       <c r="T22" s="38">
@@ -10125,7 +9818,7 @@
       <c r="Z22" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA22" s="111" t="s">
+      <c r="AA22" s="110" t="s">
         <v>994</v>
       </c>
       <c r="AB22" s="12" t="s">
@@ -10161,7 +9854,7 @@
       <c r="AL22" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM22" s="114" t="s">
+      <c r="AM22" s="113" t="s">
         <v>173</v>
       </c>
       <c r="AN22" s="28" t="s">
@@ -10325,7 +10018,7 @@
       <c r="Q24" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="R24" s="106" t="s">
+      <c r="R24" s="105" t="s">
         <v>959</v>
       </c>
       <c r="S24" s="15" t="s">
@@ -10352,7 +10045,7 @@
       <c r="Z24" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA24" s="111" t="s">
+      <c r="AA24" s="110" t="s">
         <v>995</v>
       </c>
       <c r="AB24" s="12" t="s">
@@ -10388,7 +10081,7 @@
       <c r="AL24" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AM24" s="114" t="s">
+      <c r="AM24" s="113" t="s">
         <v>187</v>
       </c>
       <c r="AN24" s="28" t="s">
@@ -10552,7 +10245,7 @@
       <c r="Q26" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R26" s="106" t="s">
+      <c r="R26" s="105" t="s">
         <v>960</v>
       </c>
       <c r="T26" s="33" t="s">
@@ -10576,7 +10269,7 @@
       <c r="Z26" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA26" s="111" t="s">
+      <c r="AA26" s="110" t="s">
         <v>995</v>
       </c>
       <c r="AB26" s="17" t="s">
@@ -10609,7 +10302,7 @@
       <c r="AL26" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM26" s="114" t="s">
+      <c r="AM26" s="113" t="s">
         <v>198</v>
       </c>
       <c r="AN26" s="28" t="s">
@@ -10776,7 +10469,7 @@
       <c r="Q28" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="R28" s="106" t="s">
+      <c r="R28" s="105" t="s">
         <v>961</v>
       </c>
       <c r="T28" s="38">
@@ -10800,7 +10493,7 @@
       <c r="Z28" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA28" s="111" t="s">
+      <c r="AA28" s="110" t="s">
         <v>996</v>
       </c>
       <c r="AB28" s="44" t="s">
@@ -10836,7 +10529,7 @@
       <c r="AL28" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM28" s="114" t="s">
+      <c r="AM28" s="113" t="s">
         <v>215</v>
       </c>
       <c r="AN28" s="28" t="s">
@@ -11000,7 +10693,7 @@
       <c r="Q30" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R30" s="106" t="s">
+      <c r="R30" s="105" t="s">
         <v>962</v>
       </c>
       <c r="T30" s="38">
@@ -11024,7 +10717,7 @@
       <c r="Z30" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA30" s="111"/>
+      <c r="AA30" s="110"/>
       <c r="AB30" s="12" t="s">
         <v>223</v>
       </c>
@@ -11058,7 +10751,7 @@
       <c r="AL30" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM30" s="114" t="s">
+      <c r="AM30" s="113" t="s">
         <v>227</v>
       </c>
       <c r="AN30" s="28" t="s">
@@ -11113,7 +10806,7 @@
       <c r="Q31" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R31" s="106" t="s">
+      <c r="R31" s="105" t="s">
         <v>962</v>
       </c>
       <c r="T31" s="38">
@@ -11137,7 +10830,7 @@
       <c r="Z31" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA31" s="111"/>
+      <c r="AA31" s="110"/>
       <c r="AB31" s="46" t="s">
         <v>232</v>
       </c>
@@ -11171,7 +10864,7 @@
       <c r="AL31" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM31" s="114" t="s">
+      <c r="AM31" s="113" t="s">
         <v>235</v>
       </c>
       <c r="AN31" s="43" t="s">
@@ -11229,7 +10922,7 @@
       <c r="Q32" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R32" s="106" t="s">
+      <c r="R32" s="105" t="s">
         <v>963</v>
       </c>
       <c r="T32" s="38">
@@ -11253,7 +10946,7 @@
       <c r="Z32" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA32" s="111"/>
+      <c r="AA32" s="110"/>
       <c r="AB32" s="46" t="s">
         <v>241</v>
       </c>
@@ -11287,7 +10980,7 @@
       <c r="AL32" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM32" s="114"/>
+      <c r="AM32" s="113"/>
       <c r="AN32" s="48" t="s">
         <v>247</v>
       </c>
@@ -11343,7 +11036,7 @@
       <c r="Q33" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R33" s="106" t="s">
+      <c r="R33" s="105" t="s">
         <v>963</v>
       </c>
       <c r="T33" s="15" t="s">
@@ -11367,7 +11060,7 @@
       <c r="Z33" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA33" s="111"/>
+      <c r="AA33" s="110"/>
       <c r="AB33" s="46" t="s">
         <v>241</v>
       </c>
@@ -11401,7 +11094,7 @@
       <c r="AL33" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM33" s="114" t="s">
+      <c r="AM33" s="113" t="s">
         <v>1023</v>
       </c>
       <c r="AN33" s="43" t="s">
@@ -11459,7 +11152,7 @@
       <c r="Q34" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R34" s="106" t="s">
+      <c r="R34" s="105" t="s">
         <v>963</v>
       </c>
       <c r="T34" s="15" t="s">
@@ -11483,7 +11176,7 @@
       <c r="Z34" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA34" s="111"/>
+      <c r="AA34" s="110"/>
       <c r="AB34" s="46" t="s">
         <v>258</v>
       </c>
@@ -11517,7 +11210,7 @@
       <c r="AL34" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM34" s="114" t="s">
+      <c r="AM34" s="113" t="s">
         <v>261</v>
       </c>
       <c r="AN34" s="50" t="s">
@@ -11575,7 +11268,7 @@
       <c r="Q35" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R35" s="106" t="s">
+      <c r="R35" s="105" t="s">
         <v>964</v>
       </c>
       <c r="T35" s="15" t="s">
@@ -11599,7 +11292,7 @@
       <c r="Z35" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA35" s="111"/>
+      <c r="AA35" s="110"/>
       <c r="AB35" s="46" t="s">
         <v>267</v>
       </c>
@@ -11633,7 +11326,7 @@
       <c r="AL35" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM35" s="114"/>
+      <c r="AM35" s="113"/>
       <c r="AN35" s="51" t="s">
         <v>271</v>
       </c>
@@ -11689,7 +11382,7 @@
       <c r="Q36" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R36" s="106" t="s">
+      <c r="R36" s="105" t="s">
         <v>964</v>
       </c>
       <c r="T36" s="15" t="s">
@@ -11713,7 +11406,7 @@
       <c r="Z36" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA36" s="111"/>
+      <c r="AA36" s="110"/>
       <c r="AB36" s="46" t="s">
         <v>274</v>
       </c>
@@ -11747,7 +11440,7 @@
       <c r="AL36" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM36" s="114" t="s">
+      <c r="AM36" s="113" t="s">
         <v>276</v>
       </c>
       <c r="AN36" s="28" t="s">
@@ -11805,7 +11498,7 @@
       <c r="Q37" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R37" s="106" t="s">
+      <c r="R37" s="105" t="s">
         <v>964</v>
       </c>
       <c r="T37" s="38">
@@ -11829,7 +11522,7 @@
       <c r="Z37" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA37" s="111"/>
+      <c r="AA37" s="110"/>
       <c r="AB37" s="44" t="s">
         <v>282</v>
       </c>
@@ -11863,7 +11556,7 @@
       <c r="AL37" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM37" s="114" t="s">
+      <c r="AM37" s="113" t="s">
         <v>284</v>
       </c>
       <c r="AN37" s="40" t="s">
@@ -11921,7 +11614,7 @@
       <c r="Q38" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="R38" s="107" t="s">
+      <c r="R38" s="106" t="s">
         <v>955</v>
       </c>
       <c r="T38" s="55" t="s">
@@ -11945,7 +11638,7 @@
       <c r="Z38" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="AA38" s="112"/>
+      <c r="AA38" s="111"/>
       <c r="AB38" s="46" t="s">
         <v>291</v>
       </c>
@@ -11979,7 +11672,7 @@
       <c r="AL38" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="AM38" s="114" t="s">
+      <c r="AM38" s="113" t="s">
         <v>294</v>
       </c>
       <c r="AN38" s="32" t="s">
@@ -12037,7 +11730,7 @@
       <c r="Q39" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R39" s="107" t="s">
+      <c r="R39" s="106" t="s">
         <v>955</v>
       </c>
       <c r="T39" s="59" t="s">
@@ -12061,7 +11754,7 @@
       <c r="Z39" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA39" s="111"/>
+      <c r="AA39" s="110"/>
       <c r="AB39" s="46" t="s">
         <v>299</v>
       </c>
@@ -12095,7 +11788,7 @@
       <c r="AL39" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM39" s="114" t="s">
+      <c r="AM39" s="113" t="s">
         <v>1022</v>
       </c>
       <c r="AN39" s="40" t="s">
@@ -12153,7 +11846,7 @@
       <c r="Q40" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R40" s="107" t="s">
+      <c r="R40" s="106" t="s">
         <v>955</v>
       </c>
       <c r="T40" s="15" t="s">
@@ -12177,7 +11870,7 @@
       <c r="Z40" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA40" s="111"/>
+      <c r="AA40" s="110"/>
       <c r="AB40" s="46" t="s">
         <v>306</v>
       </c>
@@ -12211,7 +11904,7 @@
       <c r="AL40" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM40" s="114" t="s">
+      <c r="AM40" s="113" t="s">
         <v>309</v>
       </c>
       <c r="AN40" s="40" t="s">
@@ -12269,7 +11962,7 @@
       <c r="Q41" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R41" s="106" t="s">
+      <c r="R41" s="105" t="s">
         <v>965</v>
       </c>
       <c r="S41" s="15" t="s">
@@ -12296,7 +11989,7 @@
       <c r="Z41" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA41" s="111" t="s">
+      <c r="AA41" s="110" t="s">
         <v>997</v>
       </c>
       <c r="AB41" s="59" t="s">
@@ -12332,7 +12025,7 @@
       <c r="AL41" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM41" s="114" t="s">
+      <c r="AM41" s="113" t="s">
         <v>323</v>
       </c>
       <c r="AN41" s="40" t="s">
@@ -12390,7 +12083,7 @@
       <c r="Q42" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R42" s="106" t="s">
+      <c r="R42" s="105" t="s">
         <v>965</v>
       </c>
       <c r="S42" s="15" t="s">
@@ -12417,7 +12110,7 @@
       <c r="Z42" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA42" s="111" t="s">
+      <c r="AA42" s="110" t="s">
         <v>997</v>
       </c>
       <c r="AB42" s="46" t="s">
@@ -12453,7 +12146,7 @@
       <c r="AL42" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM42" s="114" t="s">
+      <c r="AM42" s="113" t="s">
         <v>330</v>
       </c>
       <c r="AN42" s="40" t="s">
@@ -12511,7 +12204,7 @@
       <c r="Q43" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R43" s="106" t="s">
+      <c r="R43" s="105" t="s">
         <v>966</v>
       </c>
       <c r="T43" s="33" t="s">
@@ -12535,7 +12228,7 @@
       <c r="Z43" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA43" s="111"/>
+      <c r="AA43" s="110"/>
       <c r="AB43" s="46" t="s">
         <v>336</v>
       </c>
@@ -12569,7 +12262,7 @@
       <c r="AL43" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AM43" s="114" t="s">
+      <c r="AM43" s="113" t="s">
         <v>340</v>
       </c>
       <c r="AN43" s="40" t="s">
@@ -12766,9 +12459,9 @@
         <v>85</v>
       </c>
       <c r="Q46" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R46" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="R46" s="105" t="s">
         <v>967</v>
       </c>
       <c r="S46" s="15" t="s">
@@ -12795,7 +12488,7 @@
       <c r="Z46" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA46" s="111"/>
+      <c r="AA46" s="110"/>
       <c r="AB46" s="17" t="s">
         <v>349</v>
       </c>
@@ -12829,7 +12522,7 @@
       <c r="AL46" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AM46" s="114" t="s">
+      <c r="AM46" s="113" t="s">
         <v>354</v>
       </c>
       <c r="AN46" s="29" t="s">
@@ -12994,9 +12687,9 @@
         <v>85</v>
       </c>
       <c r="Q48" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R48" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="R48" s="105" t="s">
         <v>967</v>
       </c>
       <c r="S48" s="15" t="s">
@@ -13023,7 +12716,7 @@
       <c r="Z48" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA48" s="111" t="s">
+      <c r="AA48" s="110" t="s">
         <v>997</v>
       </c>
       <c r="AB48" s="12" t="s">
@@ -13059,7 +12752,7 @@
       <c r="AL48" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM48" s="114" t="s">
+      <c r="AM48" s="113" t="s">
         <v>368</v>
       </c>
       <c r="AN48" s="28" t="s">
@@ -13112,9 +12805,9 @@
         <v>56</v>
       </c>
       <c r="Q49" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R49" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="R49" s="105" t="s">
         <v>967</v>
       </c>
       <c r="S49" s="15" t="s">
@@ -13141,7 +12834,7 @@
       <c r="Z49" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA49" s="111" t="s">
+      <c r="AA49" s="110" t="s">
         <v>997</v>
       </c>
       <c r="AB49" s="63" t="s">
@@ -13174,7 +12867,7 @@
       <c r="AL49" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM49" s="114" t="s">
+      <c r="AM49" s="113" t="s">
         <v>373</v>
       </c>
       <c r="AN49" s="64" t="s">
@@ -13339,9 +13032,9 @@
         <v>56</v>
       </c>
       <c r="Q51" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R51" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="R51" s="105" t="s">
         <v>967</v>
       </c>
       <c r="S51" s="15" t="s">
@@ -13368,7 +13061,7 @@
       <c r="Z51" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA51" s="111" t="s">
+      <c r="AA51" s="110" t="s">
         <v>997</v>
       </c>
       <c r="AB51" s="63" t="s">
@@ -13401,7 +13094,7 @@
       <c r="AL51" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AM51" s="114" t="s">
+      <c r="AM51" s="113" t="s">
         <v>380</v>
       </c>
       <c r="AN51" s="64" t="s">
@@ -13675,9 +13368,9 @@
         <v>56</v>
       </c>
       <c r="Q54" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R54" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="R54" s="105" t="s">
         <v>967</v>
       </c>
       <c r="S54" s="15" t="s">
@@ -13704,7 +13397,7 @@
       <c r="Z54" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA54" s="111" t="s">
+      <c r="AA54" s="110" t="s">
         <v>998</v>
       </c>
       <c r="AB54" s="17" t="s">
@@ -13740,7 +13433,7 @@
       <c r="AL54" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AM54" s="114" t="s">
+      <c r="AM54" s="113" t="s">
         <v>391</v>
       </c>
       <c r="AN54" s="28" t="s">
@@ -13905,9 +13598,9 @@
         <v>151</v>
       </c>
       <c r="Q56" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R56" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="R56" s="105" t="s">
         <v>967</v>
       </c>
       <c r="S56" s="15" t="s">
@@ -13934,7 +13627,7 @@
       <c r="Z56" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA56" s="111" t="s">
+      <c r="AA56" s="110" t="s">
         <v>999</v>
       </c>
       <c r="AB56" s="17" t="s">
@@ -13970,7 +13663,7 @@
       <c r="AL56" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="AM56" s="114" t="s">
+      <c r="AM56" s="113" t="s">
         <v>401</v>
       </c>
       <c r="AN56" s="28" t="s">
@@ -14134,7 +13827,7 @@
       <c r="Q58" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R58" s="106" t="s">
+      <c r="R58" s="105" t="s">
         <v>968</v>
       </c>
       <c r="T58" s="38">
@@ -14158,7 +13851,7 @@
       <c r="Z58" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="AA58" s="112" t="s">
+      <c r="AA58" s="111" t="s">
         <v>1000</v>
       </c>
       <c r="AB58" s="44" t="s">
@@ -14194,7 +13887,7 @@
       <c r="AL58" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="AM58" s="114" t="s">
+      <c r="AM58" s="113" t="s">
         <v>414</v>
       </c>
       <c r="AN58" s="28" t="s">
@@ -14252,7 +13945,7 @@
       <c r="Q59" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R59" s="106" t="s">
+      <c r="R59" s="105" t="s">
         <v>968</v>
       </c>
       <c r="T59" s="15" t="s">
@@ -14276,7 +13969,7 @@
       <c r="Z59" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="AA59" s="112" t="s">
+      <c r="AA59" s="111" t="s">
         <v>1000</v>
       </c>
       <c r="AB59" s="19" t="s">
@@ -14312,7 +14005,7 @@
       <c r="AL59" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="AM59" s="114" t="s">
+      <c r="AM59" s="113" t="s">
         <v>424</v>
       </c>
       <c r="AN59" s="67" t="s">
@@ -14617,7 +14310,7 @@
       <c r="Q63" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R63" s="106" t="s">
+      <c r="R63" s="105" t="s">
         <v>969</v>
       </c>
       <c r="S63" s="15" t="s">
@@ -14644,7 +14337,7 @@
       <c r="Z63" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA63" s="111" t="s">
+      <c r="AA63" s="110" t="s">
         <v>1001</v>
       </c>
       <c r="AB63" s="17" t="s">
@@ -14680,7 +14373,7 @@
       <c r="AL63" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="AM63" s="114" t="s">
+      <c r="AM63" s="113" t="s">
         <v>448</v>
       </c>
       <c r="AN63" s="64" t="s">
@@ -14738,7 +14431,7 @@
       <c r="Q64" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="R64" s="107" t="s">
+      <c r="R64" s="106" t="s">
         <v>970</v>
       </c>
       <c r="S64" s="15" t="s">
@@ -14765,7 +14458,7 @@
       <c r="Z64" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="AA64" s="112" t="s">
+      <c r="AA64" s="111" t="s">
         <v>1002</v>
       </c>
       <c r="AB64" s="44" t="s">
@@ -14801,7 +14494,7 @@
       <c r="AL64" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="AM64" s="114" t="s">
+      <c r="AM64" s="113" t="s">
         <v>461</v>
       </c>
       <c r="AN64" s="74" t="s">
@@ -14965,7 +14658,7 @@
       <c r="Q66" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R66" s="106" t="s">
+      <c r="R66" s="105" t="s">
         <v>971</v>
       </c>
       <c r="S66" s="15" t="s">
@@ -14992,7 +14685,7 @@
       <c r="Z66" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA66" s="111" t="s">
+      <c r="AA66" s="110" t="s">
         <v>1003</v>
       </c>
       <c r="AB66" s="17" t="s">
@@ -15025,7 +14718,7 @@
       <c r="AL66" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM66" s="114" t="s">
+      <c r="AM66" s="113" t="s">
         <v>478</v>
       </c>
       <c r="AN66" s="64" t="s">
@@ -15192,7 +14885,7 @@
       <c r="Q68" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R68" s="106" t="s">
+      <c r="R68" s="105" t="s">
         <v>972</v>
       </c>
       <c r="S68" s="15" t="s">
@@ -15219,7 +14912,7 @@
       <c r="Z68" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA68" s="111" t="s">
+      <c r="AA68" s="110" t="s">
         <v>1004</v>
       </c>
       <c r="AB68" s="17" t="s">
@@ -15255,7 +14948,7 @@
       <c r="AL68" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM68" s="114" t="s">
+      <c r="AM68" s="113" t="s">
         <v>495</v>
       </c>
       <c r="AN68" s="28" t="s">
@@ -15419,7 +15112,7 @@
       <c r="Q70" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R70" s="106" t="s">
+      <c r="R70" s="105" t="s">
         <v>973</v>
       </c>
       <c r="S70" s="15" t="s">
@@ -15446,7 +15139,7 @@
       <c r="Z70" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA70" s="111" t="s">
+      <c r="AA70" s="110" t="s">
         <v>1005</v>
       </c>
       <c r="AB70" s="17" t="s">
@@ -15482,7 +15175,7 @@
       <c r="AL70" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="AM70" s="114" t="s">
+      <c r="AM70" s="113" t="s">
         <v>60</v>
       </c>
       <c r="AN70" s="28" t="s">
@@ -15537,7 +15230,7 @@
       <c r="Q71" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="R71" s="108" t="s">
+      <c r="R71" s="107" t="s">
         <v>974</v>
       </c>
       <c r="S71" s="15" t="s">
@@ -15564,7 +15257,7 @@
       <c r="Z71" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA71" s="111" t="s">
+      <c r="AA71" s="110" t="s">
         <v>1005</v>
       </c>
       <c r="AB71" s="17" t="s">
@@ -15600,7 +15293,7 @@
       <c r="AL71" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM71" s="114" t="s">
+      <c r="AM71" s="113" t="s">
         <v>511</v>
       </c>
       <c r="AN71" s="28" t="s">
@@ -15655,7 +15348,7 @@
       <c r="Q72" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R72" s="106" t="s">
+      <c r="R72" s="105" t="s">
         <v>975</v>
       </c>
       <c r="S72" s="15" t="s">
@@ -15682,7 +15375,7 @@
       <c r="Z72" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA72" s="111" t="s">
+      <c r="AA72" s="110" t="s">
         <v>1005</v>
       </c>
       <c r="AB72" s="17" t="s">
@@ -15718,7 +15411,7 @@
       <c r="AL72" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM72" s="114" t="s">
+      <c r="AM72" s="113" t="s">
         <v>517</v>
       </c>
       <c r="AN72" s="28" t="s">
@@ -15773,7 +15466,7 @@
       <c r="Q73" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R73" s="106" t="s">
+      <c r="R73" s="105" t="s">
         <v>976</v>
       </c>
       <c r="S73" s="15" t="s">
@@ -15800,7 +15493,7 @@
       <c r="Z73" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA73" s="111" t="s">
+      <c r="AA73" s="110" t="s">
         <v>1006</v>
       </c>
       <c r="AB73" s="17" t="s">
@@ -15836,7 +15529,7 @@
       <c r="AL73" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM73" s="114" t="s">
+      <c r="AM73" s="113" t="s">
         <v>527</v>
       </c>
       <c r="AN73" s="64" t="s">
@@ -16006,7 +15699,7 @@
       <c r="Q75" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="R75" s="107" t="s">
+      <c r="R75" s="106" t="s">
         <v>977</v>
       </c>
       <c r="S75" s="15" t="s">
@@ -16033,7 +15726,7 @@
       <c r="Z75" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA75" s="111" t="s">
+      <c r="AA75" s="110" t="s">
         <v>1007</v>
       </c>
       <c r="AB75" s="12" t="s">
@@ -16069,7 +15762,7 @@
       <c r="AL75" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM75" s="114" t="s">
+      <c r="AM75" s="113" t="s">
         <v>539</v>
       </c>
       <c r="AN75" s="28" t="s">
@@ -16234,7 +15927,7 @@
       <c r="Q77" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="R77" s="107" t="s">
+      <c r="R77" s="106" t="s">
         <v>1024</v>
       </c>
       <c r="S77" s="47"/>
@@ -16259,7 +15952,7 @@
       <c r="Z77" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA77" s="111" t="s">
+      <c r="AA77" s="110" t="s">
         <v>1007</v>
       </c>
       <c r="AB77" s="44" t="s">
@@ -16295,7 +15988,7 @@
       <c r="AL77" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM77" s="114" t="s">
+      <c r="AM77" s="113" t="s">
         <v>551</v>
       </c>
       <c r="AN77" s="64" t="s">
@@ -16353,7 +16046,7 @@
       <c r="Q78" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="R78" s="107" t="s">
+      <c r="R78" s="106" t="s">
         <v>1024</v>
       </c>
       <c r="S78" s="47"/>
@@ -16378,7 +16071,7 @@
       <c r="Z78" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA78" s="111"/>
+      <c r="AA78" s="110"/>
       <c r="AB78" s="63" t="s">
         <v>556</v>
       </c>
@@ -16412,7 +16105,7 @@
       <c r="AL78" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM78" s="114" t="s">
+      <c r="AM78" s="113" t="s">
         <v>561</v>
       </c>
       <c r="AN78" s="64" t="s">
@@ -16470,7 +16163,7 @@
       <c r="Q79" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R79" s="106" t="s">
+      <c r="R79" s="105" t="s">
         <v>969</v>
       </c>
       <c r="S79" s="15" t="s">
@@ -16497,7 +16190,7 @@
       <c r="Z79" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA79" s="111" t="s">
+      <c r="AA79" s="110" t="s">
         <v>1008</v>
       </c>
       <c r="AB79" s="17" t="s">
@@ -16533,7 +16226,7 @@
       <c r="AL79" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM79" s="114" t="s">
+      <c r="AM79" s="113" t="s">
         <v>572</v>
       </c>
       <c r="AN79" s="28" t="s">
@@ -16694,7 +16387,7 @@
       <c r="Q81" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="R81" s="108" t="s">
+      <c r="R81" s="107" t="s">
         <v>980</v>
       </c>
       <c r="S81" s="15" t="s">
@@ -16721,7 +16414,7 @@
       <c r="Z81" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA81" s="111" t="s">
+      <c r="AA81" s="110" t="s">
         <v>1009</v>
       </c>
       <c r="AB81" s="17" t="s">
@@ -16757,7 +16450,7 @@
       <c r="AL81" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM81" s="114" t="s">
+      <c r="AM81" s="113" t="s">
         <v>585</v>
       </c>
       <c r="AN81" s="28" t="s">
@@ -16920,9 +16613,9 @@
         <v>56</v>
       </c>
       <c r="Q83" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="R83" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="R83" s="105" t="s">
         <v>978</v>
       </c>
       <c r="S83" s="15" t="s">
@@ -16949,7 +16642,7 @@
       <c r="Z83" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA83" s="111" t="s">
+      <c r="AA83" s="110" t="s">
         <v>1007</v>
       </c>
       <c r="AB83" s="17" t="s">
@@ -16985,7 +16678,7 @@
       <c r="AL83" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM83" s="114" t="s">
+      <c r="AM83" s="113" t="s">
         <v>604</v>
       </c>
       <c r="AN83" s="64" t="s">
@@ -17043,7 +16736,7 @@
       <c r="Q84" s="24" t="s">
         <v>607</v>
       </c>
-      <c r="R84" s="108" t="s">
+      <c r="R84" s="107" t="s">
         <v>981</v>
       </c>
       <c r="S84" s="15" t="s">
@@ -17071,7 +16764,7 @@
       <c r="Z84" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA84" s="111"/>
+      <c r="AA84" s="110"/>
       <c r="AB84" s="17" t="s">
         <v>611</v>
       </c>
@@ -17105,7 +16798,7 @@
       <c r="AL84" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM84" s="114" t="s">
+      <c r="AM84" s="113" t="s">
         <v>616</v>
       </c>
       <c r="AN84" s="64" t="s">
@@ -17163,7 +16856,7 @@
       <c r="Q85" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="R85" s="109" t="s">
+      <c r="R85" s="108" t="s">
         <v>619</v>
       </c>
       <c r="S85" s="15" t="s">
@@ -17190,7 +16883,7 @@
       <c r="Z85" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="AA85" s="112" t="s">
+      <c r="AA85" s="111" t="s">
         <v>1010</v>
       </c>
       <c r="AB85" s="46" t="s">
@@ -17226,7 +16919,7 @@
       <c r="AL85" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="AM85" s="114" t="s">
+      <c r="AM85" s="113" t="s">
         <v>626</v>
       </c>
       <c r="AN85" s="67" t="s">
@@ -17391,7 +17084,7 @@
       <c r="Q87" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R87" s="106" t="s">
+      <c r="R87" s="105" t="s">
         <v>982</v>
       </c>
       <c r="S87" s="15" t="s">
@@ -17418,7 +17111,7 @@
       <c r="Z87" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA87" s="111" t="s">
+      <c r="AA87" s="110" t="s">
         <v>1009</v>
       </c>
       <c r="AB87" s="12" t="s">
@@ -17454,7 +17147,7 @@
       <c r="AL87" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM87" s="114" t="s">
+      <c r="AM87" s="113" t="s">
         <v>643</v>
       </c>
       <c r="AN87" s="64" t="s">
@@ -17512,7 +17205,7 @@
       <c r="Q88" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="R88" s="106" t="s">
+      <c r="R88" s="105" t="s">
         <v>979</v>
       </c>
       <c r="S88" s="15" t="s">
@@ -17539,7 +17232,7 @@
       <c r="Z88" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="AA88" s="112" t="s">
+      <c r="AA88" s="111" t="s">
         <v>1009</v>
       </c>
       <c r="AB88" s="46" t="s">
@@ -17575,7 +17268,7 @@
       <c r="AL88" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="AM88" s="114" t="s">
+      <c r="AM88" s="113" t="s">
         <v>657</v>
       </c>
       <c r="AN88" s="62" t="s">
@@ -17745,7 +17438,7 @@
       <c r="Q90" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R90" s="106" t="s">
+      <c r="R90" s="105" t="s">
         <v>1025</v>
       </c>
       <c r="S90" s="15" t="s">
@@ -17772,7 +17465,7 @@
       <c r="Z90" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA90" s="111" t="s">
+      <c r="AA90" s="110" t="s">
         <v>1011</v>
       </c>
       <c r="AB90" s="17" t="s">
@@ -17808,7 +17501,7 @@
       <c r="AL90" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM90" s="114" t="s">
+      <c r="AM90" s="113" t="s">
         <v>1021</v>
       </c>
       <c r="AN90" s="28" t="s">
@@ -17975,7 +17668,7 @@
       <c r="Q92" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="R92" s="106" t="s">
+      <c r="R92" s="105" t="s">
         <v>983</v>
       </c>
       <c r="S92" s="15" t="s">
@@ -18002,7 +17695,7 @@
       <c r="Z92" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA92" s="111" t="s">
+      <c r="AA92" s="110" t="s">
         <v>996</v>
       </c>
       <c r="AB92" s="12" t="s">
@@ -18038,7 +17731,7 @@
       <c r="AL92" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM92" s="114" t="s">
+      <c r="AM92" s="113" t="s">
         <v>688</v>
       </c>
       <c r="AN92" s="28" t="s">
@@ -18202,7 +17895,7 @@
       <c r="Q94" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="R94" s="106" t="s">
+      <c r="R94" s="105" t="s">
         <v>989</v>
       </c>
       <c r="T94" s="71">
@@ -18226,7 +17919,7 @@
       <c r="Z94" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="AA94" s="112" t="s">
+      <c r="AA94" s="111" t="s">
         <v>995</v>
       </c>
       <c r="AB94" s="44" t="s">
@@ -18262,7 +17955,7 @@
       <c r="AL94" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="AM94" s="114" t="s">
+      <c r="AM94" s="113" t="s">
         <v>706</v>
       </c>
       <c r="AN94" s="62" t="s">
@@ -18320,7 +18013,7 @@
       <c r="Q95" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="R95" s="106" t="s">
+      <c r="R95" s="105" t="s">
         <v>987</v>
       </c>
       <c r="T95" s="38">
@@ -18344,7 +18037,7 @@
       <c r="Z95" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA95" s="111" t="s">
+      <c r="AA95" s="110" t="s">
         <v>995</v>
       </c>
       <c r="AB95" s="17" t="s">
@@ -18380,7 +18073,7 @@
       <c r="AL95" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM95" s="114" t="s">
+      <c r="AM95" s="113" t="s">
         <v>715</v>
       </c>
       <c r="AN95" s="28" t="s">
@@ -18438,7 +18131,7 @@
       <c r="Q96" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R96" s="106" t="s">
+      <c r="R96" s="105" t="s">
         <v>984</v>
       </c>
       <c r="T96" s="38">
@@ -18462,7 +18155,7 @@
       <c r="Z96" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA96" s="111" t="s">
+      <c r="AA96" s="110" t="s">
         <v>1012</v>
       </c>
       <c r="AB96" s="17" t="s">
@@ -18498,7 +18191,7 @@
       <c r="AL96" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM96" s="114" t="s">
+      <c r="AM96" s="113" t="s">
         <v>726</v>
       </c>
       <c r="AN96" s="64" t="s">
@@ -18691,7 +18384,7 @@
       <c r="Q99" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R99" s="106" t="s">
+      <c r="R99" s="105" t="s">
         <v>985</v>
       </c>
       <c r="S99" s="15" t="s">
@@ -18718,7 +18411,7 @@
       <c r="Z99" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA99" s="111"/>
+      <c r="AA99" s="110"/>
       <c r="AB99" s="17" t="s">
         <v>738</v>
       </c>
@@ -18752,7 +18445,7 @@
       <c r="AL99" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="AM99" s="114" t="s">
+      <c r="AM99" s="113" t="s">
         <v>1020</v>
       </c>
       <c r="AN99" s="28" t="s">
@@ -18807,7 +18500,7 @@
       <c r="Q100" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R100" s="106" t="s">
+      <c r="R100" s="105" t="s">
         <v>962</v>
       </c>
       <c r="S100" s="15" t="s">
@@ -18834,7 +18527,7 @@
       <c r="Z100" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA100" s="111"/>
+      <c r="AA100" s="110"/>
       <c r="AB100" s="17" t="s">
         <v>746</v>
       </c>
@@ -18868,7 +18561,7 @@
       <c r="AL100" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="AM100" s="114" t="s">
+      <c r="AM100" s="113" t="s">
         <v>750</v>
       </c>
       <c r="AN100" s="28" t="s">
@@ -18924,7 +18617,7 @@
       <c r="Q101" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R101" s="106" t="s">
+      <c r="R101" s="105" t="s">
         <v>986</v>
       </c>
       <c r="S101" s="15" t="s">
@@ -18951,7 +18644,7 @@
       <c r="Z101" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA101" s="111"/>
+      <c r="AA101" s="110"/>
       <c r="AB101" s="17" t="s">
         <v>746</v>
       </c>
@@ -18985,7 +18678,7 @@
       <c r="AL101" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="AM101" s="114" t="s">
+      <c r="AM101" s="113" t="s">
         <v>759</v>
       </c>
       <c r="AN101" s="28" t="s">
@@ -19040,7 +18733,7 @@
       <c r="Q102" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R102" s="106" t="s">
+      <c r="R102" s="105" t="s">
         <v>1026</v>
       </c>
       <c r="S102" s="15" t="s">
@@ -19067,7 +18760,7 @@
       <c r="Z102" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA102" s="111"/>
+      <c r="AA102" s="110"/>
       <c r="AB102" s="17" t="s">
         <v>746</v>
       </c>
@@ -19101,7 +18794,7 @@
       <c r="AL102" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM102" s="114" t="s">
+      <c r="AM102" s="113" t="s">
         <v>767</v>
       </c>
       <c r="AN102" s="64" t="s">
@@ -19294,7 +18987,7 @@
       <c r="Q105" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R105" s="106" t="s">
+      <c r="R105" s="105" t="s">
         <v>962</v>
       </c>
       <c r="S105" s="15" t="s">
@@ -19321,7 +19014,7 @@
       <c r="Z105" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA105" s="111"/>
+      <c r="AA105" s="110"/>
       <c r="AB105" s="17" t="s">
         <v>738</v>
       </c>
@@ -19355,7 +19048,7 @@
       <c r="AL105" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="AM105" s="114" t="s">
+      <c r="AM105" s="113" t="s">
         <v>1019</v>
       </c>
       <c r="AN105" s="28" t="s">
@@ -19522,7 +19215,7 @@
       <c r="Q107" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R107" s="106" t="s">
+      <c r="R107" s="105" t="s">
         <v>962</v>
       </c>
       <c r="S107" s="15" t="s">
@@ -19549,7 +19242,7 @@
       <c r="Z107" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA107" s="111"/>
+      <c r="AA107" s="110"/>
       <c r="AB107" s="17" t="s">
         <v>738</v>
       </c>
@@ -19583,7 +19276,7 @@
       <c r="AL107" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="AM107" s="114" t="s">
+      <c r="AM107" s="113" t="s">
         <v>1018</v>
       </c>
       <c r="AN107" s="28" t="s">
@@ -19638,7 +19331,7 @@
       <c r="Q108" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R108" s="106" t="s">
+      <c r="R108" s="105" t="s">
         <v>962</v>
       </c>
       <c r="S108" s="15" t="s">
@@ -19665,7 +19358,7 @@
       <c r="Z108" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA108" s="111"/>
+      <c r="AA108" s="110"/>
       <c r="AB108" s="17" t="s">
         <v>738</v>
       </c>
@@ -19699,7 +19392,7 @@
       <c r="AL108" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM108" s="114" t="s">
+      <c r="AM108" s="113" t="s">
         <v>797</v>
       </c>
       <c r="AN108" s="28" t="s">
@@ -19754,7 +19447,7 @@
       <c r="Q109" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R109" s="106" t="s">
+      <c r="R109" s="105" t="s">
         <v>971</v>
       </c>
       <c r="S109" s="15" t="s">
@@ -19781,7 +19474,7 @@
       <c r="Z109" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA109" s="111"/>
+      <c r="AA109" s="110"/>
       <c r="AB109" s="17" t="s">
         <v>738</v>
       </c>
@@ -19815,7 +19508,7 @@
       <c r="AL109" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM109" s="114" t="s">
+      <c r="AM109" s="113" t="s">
         <v>805</v>
       </c>
       <c r="AN109" s="28" t="s">
@@ -19979,7 +19672,7 @@
       <c r="Q111" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R111" s="106" t="s">
+      <c r="R111" s="105" t="s">
         <v>971</v>
       </c>
       <c r="S111" s="15" t="s">
@@ -20006,7 +19699,7 @@
       <c r="Z111" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA111" s="111"/>
+      <c r="AA111" s="110"/>
       <c r="AB111" s="17" t="s">
         <v>738</v>
       </c>
@@ -20040,7 +19733,7 @@
       <c r="AL111" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM111" s="114" t="s">
+      <c r="AM111" s="113" t="s">
         <v>814</v>
       </c>
       <c r="AN111" s="28" t="s">
@@ -20095,7 +19788,7 @@
       <c r="Q112" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R112" s="106" t="s">
+      <c r="R112" s="105" t="s">
         <v>976</v>
       </c>
       <c r="S112" s="15" t="s">
@@ -20122,7 +19815,7 @@
       <c r="Z112" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA112" s="111"/>
+      <c r="AA112" s="110"/>
       <c r="AB112" s="17" t="s">
         <v>738</v>
       </c>
@@ -20156,7 +19849,7 @@
       <c r="AL112" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="AM112" s="114" t="s">
+      <c r="AM112" s="113" t="s">
         <v>822</v>
       </c>
       <c r="AN112" s="28" t="s">
@@ -20323,7 +20016,7 @@
       <c r="Q114" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R114" s="106" t="s">
+      <c r="R114" s="105" t="s">
         <v>1027</v>
       </c>
       <c r="S114" s="15" t="s">
@@ -20350,7 +20043,7 @@
       <c r="Z114" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA114" s="111"/>
+      <c r="AA114" s="110"/>
       <c r="AB114" s="17" t="s">
         <v>738</v>
       </c>
@@ -20384,7 +20077,7 @@
       <c r="AL114" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM114" s="114" t="s">
+      <c r="AM114" s="113" t="s">
         <v>836</v>
       </c>
       <c r="AN114" s="28" t="s">
@@ -20439,7 +20132,7 @@
       <c r="Q115" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="R115" s="106" t="s">
+      <c r="R115" s="105" t="s">
         <v>1028</v>
       </c>
       <c r="S115" s="15" t="s">
@@ -20466,7 +20159,7 @@
       <c r="Z115" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA115" s="111"/>
+      <c r="AA115" s="110"/>
       <c r="AB115" s="17" t="s">
         <v>738</v>
       </c>
@@ -20500,7 +20193,7 @@
       <c r="AL115" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="AM115" s="114" t="s">
+      <c r="AM115" s="113" t="s">
         <v>846</v>
       </c>
       <c r="AN115" s="75" t="s">
@@ -20693,7 +20386,7 @@
       <c r="Q118" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="R118" s="106" t="s">
+      <c r="R118" s="105" t="s">
         <v>988</v>
       </c>
       <c r="T118" s="33" t="s">
@@ -20717,7 +20410,7 @@
       <c r="Z118" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="AA118" s="111"/>
+      <c r="AA118" s="110"/>
       <c r="AB118" s="17" t="s">
         <v>860</v>
       </c>
@@ -20751,7 +20444,7 @@
       <c r="AL118" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM118" s="114" t="s">
+      <c r="AM118" s="113" t="s">
         <v>1017</v>
       </c>
       <c r="AN118" s="89" t="s">
@@ -20916,7 +20609,7 @@
       <c r="Q120" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="R120" s="106" t="s">
+      <c r="R120" s="105" t="s">
         <v>988</v>
       </c>
       <c r="T120" s="33" t="s">
@@ -20940,7 +20633,7 @@
       <c r="Z120" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA120" s="111" t="s">
+      <c r="AA120" s="110" t="s">
         <v>1013</v>
       </c>
       <c r="AB120" s="12" t="s">
@@ -20973,7 +20666,7 @@
       <c r="AL120" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM120" s="114" t="s">
+      <c r="AM120" s="113" t="s">
         <v>877</v>
       </c>
       <c r="AN120" s="39" t="s">
@@ -21031,7 +20724,7 @@
       <c r="Q121" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="R121" s="106" t="s">
+      <c r="R121" s="105" t="s">
         <v>988</v>
       </c>
       <c r="T121" s="15" t="s">
@@ -21055,7 +20748,7 @@
       <c r="Z121" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AA121" s="111" t="s">
+      <c r="AA121" s="110" t="s">
         <v>1013</v>
       </c>
       <c r="AB121" s="17" t="s">
@@ -21091,7 +20784,7 @@
       <c r="AL121" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="AM121" s="114" t="s">
+      <c r="AM121" s="113" t="s">
         <v>1017</v>
       </c>
       <c r="AN121" s="51" t="s">
@@ -21256,7 +20949,7 @@
       <c r="Q123" s="15" t="s">
         <v>607</v>
       </c>
-      <c r="R123" s="106" t="s">
+      <c r="R123" s="105" t="s">
         <v>1029</v>
       </c>
       <c r="T123" s="92" t="s">
@@ -21280,7 +20973,7 @@
       <c r="Z123" s="13" t="s">
         <v>902</v>
       </c>
-      <c r="AA123" s="111" t="s">
+      <c r="AA123" s="110" t="s">
         <v>1014</v>
       </c>
       <c r="AB123" s="12" t="s">
@@ -21316,7 +21009,7 @@
       <c r="AL123" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="AM123" s="114" t="s">
+      <c r="AM123" s="113" t="s">
         <v>1016</v>
       </c>
       <c r="AN123" s="89" t="s">
@@ -21857,1282 +21550,1282 @@
     <mergeCell ref="K1:O1"/>
   </mergeCells>
   <conditionalFormatting sqref="AH28 AH51 AH90 AH46:AH49 AH63:AH64 AH66:AH68 AH4 AH92:AH96 AP91 AK23 AI25:AJ25 AH24:AK24 AH26:AK26 AJ70:AL70 AH61:AK61 AI46:AI52 AJ46:AJ47 AI55:AI57 AI60:AK60 AI105:AK116 AI63:AI74 AJ118:AK121 AJ35 AJ36:AK38 AJ39:AJ44 AH83:AH85 AH87:AH88 AK74 AJ48:AK52 AH53:AK54 AJ55:AK59 AJ63:AK69 AJ71:AK73 AG99:AK103 AN105:AN116 AN99:AN103 AN71:AN97 AN63:AN69 AN36:AN44 AN118:AN122 AH118 AH120:AH121 AH30:AH43 AI30:AI44 AI22:AI23 AH6:AH22 AI81:AK97 AH56:AH59 AJ30:AK34 AG118:AG122 AG105:AG114 AG46:AG61 AG75:AK80 AH70:AH73 AH105:AH115 AG81:AG97 AG63:AG74 AP136:AP137 AN46:AN61 AI27:AK29 AN23:AN34 AN136:AN137 AG4:AG44 AG136:AJ137 AI118:AI123 AJ122:AJ123 AI4:AO21 AK22:AO22 AM24 AM26 AM28 AM30:AM43 AM46 AM48:AM49 AM51 AM54 AM56 AM58:AM59 AM63:AM64 AM66 AM68 AN70:AO70 AM70:AM73 AM75 AM77:AM79 AM81 AM83:AM85 AM87:AM88 AM90 AM92 AM94:AM96 AM99:AM102 AM105 AM107:AM109 AM111:AM112 AM114:AM115 AM118 AM123 AM120:AM121">
-    <cfRule type="cellIs" dxfId="293" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="261" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH5">
-    <cfRule type="cellIs" dxfId="292" priority="260" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="260" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH25">
-    <cfRule type="cellIs" dxfId="291" priority="259" operator="equal">
+    <cfRule type="cellIs" dxfId="261" priority="259" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH23">
-    <cfRule type="cellIs" dxfId="290" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="258" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ22">
-    <cfRule type="cellIs" dxfId="289" priority="257" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="257" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ23">
-    <cfRule type="cellIs" dxfId="288" priority="256" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="256" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK25">
-    <cfRule type="cellIs" dxfId="287" priority="255" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="255" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH27">
-    <cfRule type="cellIs" dxfId="286" priority="254" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="254" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH29">
-    <cfRule type="cellIs" dxfId="285" priority="253" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="253" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH50">
-    <cfRule type="cellIs" dxfId="284" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="252" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH55">
-    <cfRule type="cellIs" dxfId="283" priority="251" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="251" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH52">
-    <cfRule type="cellIs" dxfId="282" priority="250" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="250" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH65">
-    <cfRule type="cellIs" dxfId="281" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="249" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH69">
-    <cfRule type="cellIs" dxfId="280" priority="248" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="248" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH74">
-    <cfRule type="cellIs" dxfId="279" priority="247" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="247" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ74">
-    <cfRule type="cellIs" dxfId="278" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="246" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH116">
-    <cfRule type="cellIs" dxfId="277" priority="245" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="245" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH86">
-    <cfRule type="cellIs" dxfId="276" priority="244" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="244" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH91">
-    <cfRule type="cellIs" dxfId="275" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="243" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH97">
-    <cfRule type="cellIs" dxfId="274" priority="242" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="242" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH119">
-    <cfRule type="cellIs" dxfId="273" priority="241" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="241" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH122">
-    <cfRule type="cellIs" dxfId="272" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="240" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:O2 D136:J136 D99:J103 D4:J44 D46:J61 D63:J97 D105:J116 D118:J122 D141:J141">
-    <cfRule type="cellIs" dxfId="271" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="239" operator="equal">
       <formula>$B$125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI99:AJ103 AG99:AG103 AI105:AJ116 AI46:AJ61 AI63:AJ97 AG105:AG114 AG46:AG61 AG63:AG97 AG4:AG44 AG136:AG137 AI4:AJ44 AI136:AJ136 AI141:AJ141 AG118:AG124 AG141 AI118:AJ124">
-    <cfRule type="cellIs" dxfId="270" priority="262" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="262" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE123 AF118:AF123 AE114 AF114:AF116 AE105:AF113 AE99:AF103 AE63:AF97 AE46:AF61 AE4:AF44 AE135:AF137 AE124:AF124 AE141:AF141">
-    <cfRule type="cellIs" dxfId="269" priority="238" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="238" operator="equal">
       <formula>$AE$127</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE116">
-    <cfRule type="cellIs" dxfId="268" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="237" operator="equal">
       <formula>$AE$127</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF124">
-    <cfRule type="cellIs" dxfId="267" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="236" operator="equal">
       <formula>$AE$127</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE124">
-    <cfRule type="cellIs" dxfId="266" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="235" operator="equal">
       <formula>$AE$127</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN119:AN122">
-    <cfRule type="cellIs" dxfId="265" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="234" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK39:AK44">
-    <cfRule type="cellIs" dxfId="264" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="233" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK46:AK47">
-    <cfRule type="cellIs" dxfId="263" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="232" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL23:AM23">
-    <cfRule type="cellIs" dxfId="262" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="231" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO23">
-    <cfRule type="cellIs" dxfId="261" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="230" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL24">
-    <cfRule type="cellIs" dxfId="260" priority="229" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="229" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL25:AM25">
-    <cfRule type="cellIs" dxfId="259" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="228" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL26">
-    <cfRule type="cellIs" dxfId="258" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="227" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL27:AM27">
-    <cfRule type="cellIs" dxfId="257" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="226" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL28">
-    <cfRule type="cellIs" dxfId="256" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="225" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL29:AM29">
-    <cfRule type="cellIs" dxfId="255" priority="224" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="224" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL30">
-    <cfRule type="cellIs" dxfId="254" priority="223" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="223" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL63">
-    <cfRule type="cellIs" dxfId="253" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="205" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL33">
-    <cfRule type="cellIs" dxfId="252" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="222" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL36">
-    <cfRule type="cellIs" dxfId="251" priority="221" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="221" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL65:AM65">
-    <cfRule type="cellIs" dxfId="250" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="204" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL38">
-    <cfRule type="cellIs" dxfId="249" priority="220" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="220" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL40">
-    <cfRule type="cellIs" dxfId="248" priority="219" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="219" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL42">
-    <cfRule type="cellIs" dxfId="247" priority="218" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="218" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL43">
-    <cfRule type="cellIs" dxfId="246" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="217" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL44:AM44">
-    <cfRule type="cellIs" dxfId="245" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="216" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL46">
-    <cfRule type="cellIs" dxfId="244" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="215" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL47:AM47">
-    <cfRule type="cellIs" dxfId="243" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="214" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL48">
-    <cfRule type="cellIs" dxfId="242" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="213" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL71">
-    <cfRule type="cellIs" dxfId="241" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="198" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL51">
-    <cfRule type="cellIs" dxfId="240" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="212" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL53:AM53">
-    <cfRule type="cellIs" dxfId="239" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="211" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL54">
-    <cfRule type="cellIs" dxfId="238" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="210" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL56">
-    <cfRule type="cellIs" dxfId="237" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="209" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL57:AM57">
-    <cfRule type="cellIs" dxfId="236" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="208" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL58">
-    <cfRule type="cellIs" dxfId="235" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="207" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL60:AM60">
-    <cfRule type="cellIs" dxfId="234" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="206" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL64">
-    <cfRule type="cellIs" dxfId="233" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="203" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL66">
-    <cfRule type="cellIs" dxfId="232" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="202" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL67:AM67">
-    <cfRule type="cellIs" dxfId="231" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="201" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL68">
-    <cfRule type="cellIs" dxfId="230" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="200" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL69:AM69">
-    <cfRule type="cellIs" dxfId="229" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="199" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL72">
-    <cfRule type="cellIs" dxfId="228" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="197" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL73">
-    <cfRule type="cellIs" dxfId="227" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="196" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL74:AM74">
-    <cfRule type="cellIs" dxfId="226" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="195" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL75">
-    <cfRule type="cellIs" dxfId="225" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="194" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL76:AM76">
-    <cfRule type="cellIs" dxfId="224" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="193" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL77">
-    <cfRule type="cellIs" dxfId="223" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="192" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL78">
-    <cfRule type="cellIs" dxfId="222" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="191" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL79">
-    <cfRule type="cellIs" dxfId="221" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="190" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL80:AM80">
-    <cfRule type="cellIs" dxfId="220" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="189" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL81">
-    <cfRule type="cellIs" dxfId="219" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="188" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL83">
-    <cfRule type="cellIs" dxfId="218" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="187" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL82:AM82">
-    <cfRule type="cellIs" dxfId="217" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="186" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL84">
-    <cfRule type="cellIs" dxfId="216" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="185" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL85">
-    <cfRule type="cellIs" dxfId="215" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="184" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL86:AM86">
-    <cfRule type="cellIs" dxfId="214" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="183" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL89:AM89">
-    <cfRule type="cellIs" dxfId="213" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="182" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL90">
-    <cfRule type="cellIs" dxfId="212" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="181" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL91:AM91">
-    <cfRule type="cellIs" dxfId="211" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="180" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL92">
-    <cfRule type="cellIs" dxfId="210" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="179" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL93:AM93">
-    <cfRule type="cellIs" dxfId="209" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="178" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL94">
-    <cfRule type="cellIs" dxfId="208" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="177" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL101">
-    <cfRule type="cellIs" dxfId="207" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="173" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL97:AM97">
-    <cfRule type="cellIs" dxfId="206" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="176" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL99">
-    <cfRule type="cellIs" dxfId="205" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="175" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL100">
-    <cfRule type="cellIs" dxfId="204" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="174" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL105">
-    <cfRule type="cellIs" dxfId="203" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="171" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL103:AM103">
-    <cfRule type="cellIs" dxfId="202" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="172" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL106:AM106">
-    <cfRule type="cellIs" dxfId="201" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="170" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL107">
-    <cfRule type="cellIs" dxfId="200" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="169" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL108">
-    <cfRule type="cellIs" dxfId="199" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="168" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL109">
-    <cfRule type="cellIs" dxfId="198" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="167" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL110:AM110">
-    <cfRule type="cellIs" dxfId="197" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="166" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL111">
-    <cfRule type="cellIs" dxfId="196" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="165" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL112">
-    <cfRule type="cellIs" dxfId="195" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="164" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL113:AM113">
-    <cfRule type="cellIs" dxfId="194" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="163" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL114">
-    <cfRule type="cellIs" dxfId="193" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="162" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL115">
-    <cfRule type="cellIs" dxfId="192" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="161" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL116:AM116">
-    <cfRule type="cellIs" dxfId="191" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="160" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL120">
-    <cfRule type="cellIs" dxfId="190" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="159" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL123">
-    <cfRule type="cellIs" dxfId="189" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="158" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL124:AM124">
-    <cfRule type="cellIs" dxfId="188" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="157" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO124">
-    <cfRule type="cellIs" dxfId="187" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="156" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO123">
-    <cfRule type="cellIs" dxfId="186" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="155" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL141:AM141">
-    <cfRule type="cellIs" dxfId="185" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="154" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO141">
-    <cfRule type="cellIs" dxfId="184" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="153" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL118">
-    <cfRule type="cellIs" dxfId="183" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="152" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO118">
-    <cfRule type="cellIs" dxfId="182" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="151" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL121">
-    <cfRule type="cellIs" dxfId="181" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="150" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL122:AM122">
-    <cfRule type="cellIs" dxfId="180" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="149" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO122">
-    <cfRule type="cellIs" dxfId="179" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="148" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO121">
-    <cfRule type="cellIs" dxfId="178" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="147" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO120">
-    <cfRule type="cellIs" dxfId="177" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="146" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO116">
-    <cfRule type="cellIs" dxfId="176" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="145" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO115">
-    <cfRule type="cellIs" dxfId="175" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="144" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO113">
-    <cfRule type="cellIs" dxfId="174" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="143" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO112">
-    <cfRule type="cellIs" dxfId="173" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="142" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO111">
-    <cfRule type="cellIs" dxfId="172" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="141" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO110">
-    <cfRule type="cellIs" dxfId="171" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="140" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO109">
-    <cfRule type="cellIs" dxfId="170" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="139" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO108">
-    <cfRule type="cellIs" dxfId="169" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="138" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO114">
-    <cfRule type="cellIs" dxfId="168" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="137" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO107">
-    <cfRule type="cellIs" dxfId="167" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="136" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO106">
-    <cfRule type="cellIs" dxfId="166" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="135" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO105">
-    <cfRule type="cellIs" dxfId="165" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="134" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO103">
-    <cfRule type="cellIs" dxfId="164" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="133" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO101">
-    <cfRule type="cellIs" dxfId="163" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="132" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO100">
-    <cfRule type="cellIs" dxfId="162" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="131" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO99">
-    <cfRule type="cellIs" dxfId="161" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="130" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO97">
-    <cfRule type="cellIs" dxfId="160" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="129" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO93">
-    <cfRule type="cellIs" dxfId="159" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="127" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO95">
-    <cfRule type="cellIs" dxfId="158" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="128" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO92">
-    <cfRule type="cellIs" dxfId="157" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="126" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO91">
-    <cfRule type="cellIs" dxfId="156" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="125" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO90">
-    <cfRule type="cellIs" dxfId="155" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="124" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO89">
-    <cfRule type="cellIs" dxfId="154" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="123" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO76">
-    <cfRule type="cellIs" dxfId="153" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="114" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO86">
-    <cfRule type="cellIs" dxfId="152" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="122" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO85">
-    <cfRule type="cellIs" dxfId="151" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="121" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO84">
-    <cfRule type="cellIs" dxfId="150" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="120" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO83">
-    <cfRule type="cellIs" dxfId="149" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="119" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO81">
-    <cfRule type="cellIs" dxfId="148" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="118" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO80">
-    <cfRule type="cellIs" dxfId="147" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="117" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO79">
-    <cfRule type="cellIs" dxfId="146" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="116" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO66">
-    <cfRule type="cellIs" dxfId="145" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="106" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO77">
-    <cfRule type="cellIs" dxfId="144" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="115" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO75">
-    <cfRule type="cellIs" dxfId="143" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="113" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO74">
-    <cfRule type="cellIs" dxfId="142" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="112" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO58">
-    <cfRule type="cellIs" dxfId="141" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="100" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO72">
-    <cfRule type="cellIs" dxfId="140" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="111" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO71">
-    <cfRule type="cellIs" dxfId="139" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="110" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO69">
-    <cfRule type="cellIs" dxfId="138" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="109" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO68">
-    <cfRule type="cellIs" dxfId="137" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="108" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO67">
-    <cfRule type="cellIs" dxfId="136" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="107" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO65">
-    <cfRule type="cellIs" dxfId="135" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="105" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO64">
-    <cfRule type="cellIs" dxfId="134" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="104" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO63">
-    <cfRule type="cellIs" dxfId="133" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="103" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO61">
-    <cfRule type="cellIs" dxfId="132" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="102" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO60">
-    <cfRule type="cellIs" dxfId="131" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="101" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO57">
-    <cfRule type="cellIs" dxfId="130" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="99" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO56">
-    <cfRule type="cellIs" dxfId="129" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="98" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO54">
-    <cfRule type="cellIs" dxfId="128" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="97" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO53">
-    <cfRule type="cellIs" dxfId="127" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="96" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO34">
-    <cfRule type="cellIs" dxfId="126" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="86" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO48">
-    <cfRule type="cellIs" dxfId="125" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="95" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO46">
-    <cfRule type="cellIs" dxfId="124" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="94" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO44">
-    <cfRule type="cellIs" dxfId="123" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="93" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO43">
-    <cfRule type="cellIs" dxfId="122" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="92" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO42">
-    <cfRule type="cellIs" dxfId="121" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="91" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO41">
-    <cfRule type="cellIs" dxfId="120" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="90" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO40">
-    <cfRule type="cellIs" dxfId="119" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="89" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO82">
-    <cfRule type="cellIs" dxfId="118" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="74" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO38">
-    <cfRule type="cellIs" dxfId="117" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="88" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO36">
-    <cfRule type="cellIs" dxfId="116" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="87" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO33">
-    <cfRule type="cellIs" dxfId="115" priority="85" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="85" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO47">
-    <cfRule type="cellIs" dxfId="114" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="63" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO30">
-    <cfRule type="cellIs" dxfId="113" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="84" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO29">
-    <cfRule type="cellIs" dxfId="112" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="83" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO28">
-    <cfRule type="cellIs" dxfId="111" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="82" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO27">
-    <cfRule type="cellIs" dxfId="110" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="81" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO26">
-    <cfRule type="cellIs" dxfId="109" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="80" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO25">
-    <cfRule type="cellIs" dxfId="108" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="79" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO24">
-    <cfRule type="cellIs" dxfId="107" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="78" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL119:AM119">
-    <cfRule type="cellIs" dxfId="106" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="77" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK122">
-    <cfRule type="cellIs" dxfId="105" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="76" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK122">
-    <cfRule type="cellIs" dxfId="104" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO119">
-    <cfRule type="cellIs" dxfId="103" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="73" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL136:AM136">
-    <cfRule type="cellIs" dxfId="102" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="72" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO136">
-    <cfRule type="cellIs" dxfId="101" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="71" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D137:J137">
-    <cfRule type="cellIs" dxfId="100" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="69" operator="equal">
       <formula>$B$125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI137:AJ137">
-    <cfRule type="cellIs" dxfId="99" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="70" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL137:AM137">
-    <cfRule type="cellIs" dxfId="98" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="67" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO137">
-    <cfRule type="cellIs" dxfId="97" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="66" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL32">
-    <cfRule type="cellIs" dxfId="96" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="65" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO32">
-    <cfRule type="cellIs" dxfId="95" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="64" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH81">
-    <cfRule type="cellIs" dxfId="94" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="62" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH44">
-    <cfRule type="cellIs" dxfId="93" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="61" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL59">
-    <cfRule type="cellIs" dxfId="92" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="60" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO59">
-    <cfRule type="cellIs" dxfId="91" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="59" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH60">
-    <cfRule type="cellIs" dxfId="90" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="58" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE115">
-    <cfRule type="cellIs" dxfId="89" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="57" operator="equal">
       <formula>$AE$127</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH89">
-    <cfRule type="cellIs" dxfId="88" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="56" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL61:AM61">
-    <cfRule type="cellIs" dxfId="87" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="55" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG137">
-    <cfRule type="cellIs" dxfId="86" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="54" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH82">
-    <cfRule type="cellIs" dxfId="85" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="53" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL35">
-    <cfRule type="cellIs" dxfId="84" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="52" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO35">
-    <cfRule type="cellIs" dxfId="83" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="51" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL50:AM50">
-    <cfRule type="cellIs" dxfId="82" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="50" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO50">
-    <cfRule type="cellIs" dxfId="81" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="49" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL52:AM52">
-    <cfRule type="cellIs" dxfId="80" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="48" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO52">
-    <cfRule type="cellIs" dxfId="79" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL55:AM55">
-    <cfRule type="cellIs" dxfId="78" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="46" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO55">
-    <cfRule type="cellIs" dxfId="77" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI99:AI103 AG99:AG103 AI105:AI116 AI46:AI61 AI63:AI97 AG105:AG114 AG46:AG61 AG63:AG97 AG4:AG44 AI4:AI44 AG135:AG137 AJ15 AI135:AI137 AI141 AG118:AG124 AG141 AI118:AI124 AJ123">
-    <cfRule type="cellIs" dxfId="76" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="43" operator="equal">
       <formula>$AI$135</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46:C61 C99:C103 C105:C116 C63:C97 W46:Y61 V40:V61 T40:U40 T39:V39 C4:C44 W22:Y44 AB9:AB12 AB14:AB15 AB17:AB21 C135:C137 P1:Y2 P135:Y137 C141 P141:Y141 P118:Y124 C118:C124 P39:S40 P4:Y21 P22:V38 P41:U44 P46:U61 P99:Y103 P105:Y116 P63:Y97">
-    <cfRule type="cellIs" dxfId="75" priority="42" operator="equal">
+  <conditionalFormatting sqref="C46:C61 C99:C103 C105:C116 C63:C97 W46:Y61 V40:V61 T40:U40 T39:V39 C4:C44 W22:Y44 AB9:AB12 AB14:AB15 AB17:AB21 C135:C137 P1:Y2 P135:Y137 C141 P141:Y141 P118:Y124 C118:C124 P39:S40 P4:Y21 P22:V38 P41:U44 P99:Y103 P105:Y116 P63:Y97 P46:U61">
+    <cfRule type="cellIs" dxfId="45" priority="42" operator="equal">
       <formula>$B$135</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D135:J135">
-    <cfRule type="cellIs" dxfId="74" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="41" operator="equal">
       <formula>$B$125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI135:AJ135 AG135">
-    <cfRule type="cellIs" dxfId="73" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q135:AB135 Q1:AC2 W41:AA41 W40:AB40 W77:AB77 W79:AB79 W78:AA78 V40:V61 W63:AC63 W64:AB64 W43:AC44 W42:AB42 T40:U40 AB74:AB75 Q76:AB76 AB89:AB97 Q17:Y29 T39:AB39 AC105:AC114 AC46:AC61 Q136:AC137 AC30:AC42 Z17:AB28 AC4:AC28 Z29:AC29 W46:AB48 W53:AB61 Z74:AA74 Q89:AA89 Q118:AB124 Q141:AB141 AC64:AC97 Q39:S40 Q41:U44 Q46:U61 Q90:Y97 Q63:V64 Q65:AB73 Q74:Y75 Q80:AB88 Q99:AC103 Q105:AB116 Q4:AB16 Q30:AB38 W49:AA52 Q77:V79">
-    <cfRule type="cellIs" dxfId="72" priority="40" operator="equal">
+  <conditionalFormatting sqref="Q135:AB135 Q1:AC2 W41:AA41 W40:AB40 W77:AB77 W79:AB79 W78:AA78 V40:V61 W63:AC63 W64:AB64 W43:AC44 W42:AB42 T40:U40 AB74:AB75 Q76:AB76 AB89:AB97 Q17:Y29 T39:AB39 AC105:AC114 AC46:AC61 Q136:AC137 AC30:AC42 Z17:AB28 AC4:AC28 Z29:AC29 W46:AB48 W53:AB61 Z74:AA74 Q89:AA89 Q118:AB124 Q141:AB141 AC64:AC97 Q39:S40 Q41:U44 Q90:Y97 Q63:V64 Q65:AB73 Q74:Y75 Q80:AB88 Q99:AC103 Q105:AB116 Q4:AB16 Q30:AB38 W49:AA52 Q77:V79 Q46:U61">
+    <cfRule type="cellIs" dxfId="42" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL135:AM135">
-    <cfRule type="cellIs" dxfId="71" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="38" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO135">
-    <cfRule type="cellIs" dxfId="70" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="37" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI137">
-    <cfRule type="cellIs" dxfId="69" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI137">
-    <cfRule type="cellIs" dxfId="68" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z75:AA75">
-    <cfRule type="cellIs" dxfId="67" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE118:AE122">
-    <cfRule type="cellIs" dxfId="66" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
       <formula>$AE$127</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E123:J123">
-    <cfRule type="cellIs" dxfId="65" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="32" operator="equal">
       <formula>$B$135</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E124:J124">
-    <cfRule type="cellIs" dxfId="64" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="31" operator="equal">
       <formula>$B$135</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL31">
-    <cfRule type="cellIs" dxfId="63" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO31">
-    <cfRule type="cellIs" dxfId="62" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="29" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL34">
-    <cfRule type="cellIs" dxfId="61" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="28" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL37">
-    <cfRule type="cellIs" dxfId="60" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO37">
-    <cfRule type="cellIs" dxfId="59" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="26" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL39">
-    <cfRule type="cellIs" dxfId="58" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO39">
-    <cfRule type="cellIs" dxfId="57" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="24" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL41">
-    <cfRule type="cellIs" dxfId="56" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="23" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL49">
-    <cfRule type="cellIs" dxfId="55" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="22" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO49">
-    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO51">
-    <cfRule type="cellIs" dxfId="53" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO73">
-    <cfRule type="cellIs" dxfId="52" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO78">
-    <cfRule type="cellIs" dxfId="51" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO87">
-    <cfRule type="cellIs" dxfId="50" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="17" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO88">
-    <cfRule type="cellIs" dxfId="49" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL87">
-    <cfRule type="cellIs" dxfId="48" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL88">
-    <cfRule type="cellIs" dxfId="47" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO94">
-    <cfRule type="cellIs" dxfId="46" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL95">
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL96">
-    <cfRule type="cellIs" dxfId="44" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO96">
-    <cfRule type="cellIs" dxfId="43" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL102">
-    <cfRule type="cellIs" dxfId="42" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO102">
-    <cfRule type="cellIs" dxfId="41" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>$AP$1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:O2">
-    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>$A$73</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123">
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
       <formula>$B$125</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D124">
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>$B$125</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>